<commit_message>
Fixed minor BOM and Footprint issues
</commit_message>
<xml_diff>
--- a/Acquisition-System/Project Outputs for Audio-Beamformer/Acquisition-System_V1.0 BOM.xlsx
+++ b/Acquisition-System/Project Outputs for Audio-Beamformer/Acquisition-System_V1.0 BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\GoogleDrive\MSE\PA-OST-2023\heron-hardware\Acquisition-System\Project Outputs for Audio-Beamformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE3B82B-17D7-444F-99A4-04E018654644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16F7A81-4E68-416B-A893-42B6D8395479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,7 +97,7 @@
     <t>270 (75V, 100mW, 1%)</t>
   </si>
   <si>
-    <t>SKRPACE010</t>
+    <t>EVQQ2U02W</t>
   </si>
   <si>
     <t>Ø 2.54mm (Black)</t>
@@ -373,7 +373,7 @@
     <t>C22966</t>
   </si>
   <si>
-    <t>C139797</t>
+    <t>C395227</t>
   </si>
   <si>
     <t>C238122</t>
@@ -772,13 +772,13 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>